<commit_message>
se agrego ejemplo de diagama de CRUD
</commit_message>
<xml_diff>
--- a/proyectoBAR/1-PlanificacionSeguimientoYControl/Planificación.xlsx
+++ b/proyectoBAR/1-PlanificacionSeguimientoYControl/Planificación.xlsx
@@ -16,21 +16,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Planificacion del proyecto BAR</t>
   </si>
   <si>
-    <t>fecaha</t>
-  </si>
-  <si>
     <t>tarea</t>
   </si>
   <si>
     <t>responsables</t>
   </si>
   <si>
-    <t>Analisis de requerimiento -FADA</t>
+    <t>Analisis de requerimiento -FODA</t>
+  </si>
+  <si>
+    <t>todos</t>
+  </si>
+  <si>
+    <t>fecha incio</t>
+  </si>
+  <si>
+    <t>fecha fin</t>
+  </si>
+  <si>
+    <t>Conseguir un cliente</t>
+  </si>
+  <si>
+    <t>Buscar productos relacionados directamente</t>
+  </si>
+  <si>
+    <t>Buscar productos relacionados indirectamente</t>
+  </si>
+  <si>
+    <t>Lima</t>
+  </si>
+  <si>
+    <t>Lima, Gomez</t>
+  </si>
+  <si>
+    <t>Engers</t>
+  </si>
+  <si>
+    <t>Establecer Vision</t>
   </si>
 </sst>
 </file>
@@ -363,41 +390,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>45518</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1">
+        <v>45518</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>45518</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45596</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="1">
+        <v>45596</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="1">
+        <v>45596</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="1">
+        <v>45561</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>